<commit_message>
Completa la primera práctica de Excel
</commit_message>
<xml_diff>
--- a/PrimerEjercicio.xlsx
+++ b/PrimerEjercicio.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yosoy\OneDrive\Escritorio\Excel Practicas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34CE8CA-8DA3-4DDF-BC21-A94123B30F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,68 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Ramiro</t>
+  </si>
+  <si>
+    <t>Denisse</t>
+  </si>
+  <si>
+    <t>Cesar</t>
+  </si>
+  <si>
+    <t>Gerardo</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Ramiro Enero</t>
+  </si>
+  <si>
+    <t>Denisse Febrero</t>
+  </si>
+  <si>
+    <t>Cesar Marzo</t>
+  </si>
+  <si>
+    <t>Gerardo Abril</t>
+  </si>
+  <si>
+    <t>Luis Mayo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,6 +128,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>218286</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>65809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1332F559-F9A5-EF73-BCC6-30E2D8B35D78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="0"/>
+          <a:ext cx="6314286" cy="6923809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +441,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Crea tu primer libro
</commit_message>
<xml_diff>
--- a/PrimerEjercicio.xlsx
+++ b/PrimerEjercicio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yosoy\OneDrive\Escritorio\Excel Practicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34CE8CA-8DA3-4DDF-BC21-A94123B30F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E98F16-9971-4C92-8744-81B237D6F34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,12 +107,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +461,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,57 +470,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>